<commit_message>
Uploading to git for backup purposes
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amberwessels/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mediacollegeamsterdam-my.sharepoint.com/personal/35741_ma-web_nl/Documents/Personal/06 Persoonlijke documenten/09 Stage/03 DTT/Assessment DTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFE4BF53-09D2-BD4D-ADBD-B4C82922A991}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="34620" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Subject</t>
   </si>
@@ -48,31 +48,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example 1</t>
-  </si>
-  <si>
-    <t>Implementing …</t>
-  </si>
-  <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
-  </si>
-  <si>
     <t>Total amount of hours</t>
   </si>
   <si>
     <t>Bonus</t>
-  </si>
-  <si>
-    <t>Example 3</t>
-  </si>
-  <si>
-    <t>Implemented bonus feature….</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <r>
@@ -95,6 +74,18 @@
       <t xml:space="preserve"> 
 Fill in the number of hours that were required to complete the test. Please include every step you took during the process and include a detailed description of every step. Add reasoning on why you took certain decisions or applied specific techniques. We prefer quality over quantity so take your time with the test and the log.</t>
     </r>
+  </si>
+  <si>
+    <t>Creating Project Folder Structure</t>
+  </si>
+  <si>
+    <t>Created the folder structure of the Vue App.</t>
+  </si>
+  <si>
+    <t>Creating basic structure of project itself</t>
+  </si>
+  <si>
+    <t>Started creating all the files needed for the project and started working with components</t>
   </si>
 </sst>
 </file>
@@ -398,10 +389,10 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1708,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1732,7 +1723,7 @@
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1754,58 +1745,48 @@
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="18">
-        <v>42736</v>
+        <v>45237</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="18">
-        <v>42736</v>
+        <v>45240</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="17">
-        <v>5</v>
-      </c>
-      <c r="C6" s="18">
-        <v>42736</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="19"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1994,11 +1975,11 @@
     </row>
     <row r="30" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Pushing changes of the last week to github
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mediacollegeamsterdam-my.sharepoint.com/personal/35741_ma-web_nl/Documents/Personal/06 Persoonlijke documenten/09 Stage/03 DTT/Assessment DTT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashlaysteur/Library/CloudStorage/OneDrive-MediacollegeAmsterdam/Personal/06 Persoonlijke documenten/09 Stage/03 DTT/Assessment DTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFE4BF53-09D2-BD4D-ADBD-B4C82922A991}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67DBCC4-E3D1-8848-9508-E7F5EA094D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Subject</t>
   </si>
@@ -85,7 +85,31 @@
     <t>Creating basic structure of project itself</t>
   </si>
   <si>
-    <t>Started creating all the files needed for the project and started working with components</t>
+    <t>Continue working on houseList and filterComponent</t>
+  </si>
+  <si>
+    <t>Continue working on houseList and HomeView</t>
+  </si>
+  <si>
+    <t>Fixing errors that were causing things to render incorrectly. Also added button for sorting.</t>
+  </si>
+  <si>
+    <t>Working on sorting and filtering</t>
+  </si>
+  <si>
+    <t>Fixing some bugs that caused the site to be unable to sort or filter houses based on the users input.</t>
+  </si>
+  <si>
+    <t>Continued working on filterComponent, houseList and homeView to make evertything work as expected.</t>
+  </si>
+  <si>
+    <t>Started creating all the files needed for the project and started working with components.</t>
+  </si>
+  <si>
+    <t>Adding create new button and page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding button for creating new house, also added the page where you can create that new house. </t>
   </si>
 </sst>
 </file>
@@ -1699,16 +1723,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="172" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.625" style="1" customWidth="1"/>
     <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
     <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
@@ -1776,40 +1800,72 @@
         <v>45240</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
+      <c r="A6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>45242</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>45245</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18">
+        <v>45246</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="17">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18">
+        <v>45247</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
@@ -1979,7 +2035,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Updated hour log uploaded
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashlaysteur/Library/CloudStorage/OneDrive-MediacollegeAmsterdam/Personal/06 Persoonlijke documenten/09 Stage/03 DTT/Assessment DTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BE8815A-1932-3F46-85CF-565276121A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BA26324-74ED-5D4B-89E8-6E40398B01E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Subject</t>
   </si>
@@ -167,6 +167,36 @@
   </si>
   <si>
     <t>Added the feautue that you can now add a house to your list of favorites, so that you can keep it and show it to your friends</t>
+  </si>
+  <si>
+    <t>Fixed error regarding formCpomponent and changed components names</t>
+  </si>
+  <si>
+    <t>Fixed error that meant tht editing was disabled, changed xomponents names and removed unused variables</t>
+  </si>
+  <si>
+    <t>Fixing erorr with formComponent and updated the API part of the site</t>
+  </si>
+  <si>
+    <t>Fixed error of editing part that came back, also removed the data.vue and added API.js</t>
+  </si>
+  <si>
+    <t>Changed all the API calls from using the methods in vue to use the js file</t>
+  </si>
+  <si>
+    <t>Changed API calls to use the js file instead of the vue file</t>
+  </si>
+  <si>
+    <t>Fixed error with showing houses as a card and in detail form</t>
+  </si>
+  <si>
+    <t>Changing the way empty housenumberAdditions are treated inside the website</t>
+  </si>
+  <si>
+    <t>Fixing styling errors that came up by changing the way that the websites worked</t>
+  </si>
+  <si>
+    <t>Fixed the bugs that showed on the screen due to it being different then first, Including formComponent and other files</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1825,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2093,42 +2123,82 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="15"/>
+      <c r="A19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="17">
+        <v>1</v>
+      </c>
+      <c r="C19" s="18">
+        <v>45273</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="15"/>
+      <c r="A20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="17">
+        <v>4</v>
+      </c>
+      <c r="C20" s="18">
+        <v>45278</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="15"/>
+      <c r="A21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="17">
+        <v>2</v>
+      </c>
+      <c r="C21" s="18">
+        <v>45279</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="15"/>
+      <c r="A22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="18">
+        <v>45280</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
+      <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="17">
+        <v>1</v>
+      </c>
+      <c r="C23" s="18">
+        <v>45281</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
@@ -2178,7 +2248,7 @@
       </c>
       <c r="B29" s="14">
         <f>SUMIF(E4:E27,"&lt;&gt;x",B4:B27)</f>
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>

</xml_diff>